<commit_message>
Feel rus discr 1
</commit_message>
<xml_diff>
--- a/IMSConfigurator/IMSConfigurator/138-2018 Kraftway.xlsx
+++ b/IMSConfigurator/IMSConfigurator/138-2018 Kraftway.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\MAINSERVER\Common\SALES\PRIME TIME new\Коммерческие предложения\2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\IMS\IMSConfigurator\IMSConfigurator\IMSConfigurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -715,6 +715,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="14" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -724,25 +730,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1460,8 +1460,8 @@
   </sheetPr>
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1699,7 +1699,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="42" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="80">
+      <c r="A21" s="86">
         <v>1</v>
       </c>
       <c r="B21" s="69" t="s">
@@ -1708,131 +1708,131 @@
       <c r="C21" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="77">
+      <c r="D21" s="79">
         <v>1</v>
       </c>
-      <c r="E21" s="81">
+      <c r="E21" s="82">
         <v>18076</v>
       </c>
-      <c r="F21" s="82">
+      <c r="F21" s="85">
         <f>E21*D21</f>
         <v>18076</v>
       </c>
       <c r="G21" s="46"/>
     </row>
     <row r="22" spans="1:7" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="78"/>
+      <c r="A22" s="80"/>
       <c r="B22" s="76" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="78"/>
+      <c r="D22" s="80"/>
       <c r="E22" s="83"/>
       <c r="F22" s="83"/>
       <c r="G22" s="46"/>
     </row>
     <row r="23" spans="1:7" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="78"/>
+      <c r="A23" s="80"/>
       <c r="B23" s="76" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="78"/>
+      <c r="D23" s="80"/>
       <c r="E23" s="83"/>
       <c r="F23" s="83"/>
       <c r="G23" s="46"/>
     </row>
     <row r="24" spans="1:7" s="42" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="78"/>
+      <c r="A24" s="80"/>
       <c r="B24" s="76" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="78"/>
+      <c r="D24" s="80"/>
       <c r="E24" s="83"/>
       <c r="F24" s="83"/>
       <c r="G24" s="46"/>
     </row>
     <row r="25" spans="1:7" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="78"/>
+      <c r="A25" s="80"/>
       <c r="B25" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="78"/>
+      <c r="D25" s="80"/>
       <c r="E25" s="83"/>
       <c r="F25" s="83"/>
       <c r="G25" s="46"/>
     </row>
     <row r="26" spans="1:7" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="78"/>
+      <c r="A26" s="80"/>
       <c r="B26" s="76" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="78"/>
+      <c r="D26" s="80"/>
       <c r="E26" s="83"/>
       <c r="F26" s="83"/>
       <c r="G26" s="46"/>
     </row>
     <row r="27" spans="1:7" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="78"/>
+      <c r="A27" s="80"/>
       <c r="B27" s="76" t="s">
         <v>45</v>
       </c>
       <c r="C27" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="78"/>
+      <c r="D27" s="80"/>
       <c r="E27" s="83"/>
       <c r="F27" s="83"/>
       <c r="G27" s="46"/>
     </row>
     <row r="28" spans="1:7" s="42" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="78"/>
+      <c r="A28" s="80"/>
       <c r="B28" s="76" t="s">
         <v>47</v>
       </c>
       <c r="C28" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="78"/>
+      <c r="D28" s="80"/>
       <c r="E28" s="83"/>
       <c r="F28" s="83"/>
       <c r="G28" s="46"/>
     </row>
     <row r="29" spans="1:7" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="78"/>
+      <c r="A29" s="80"/>
       <c r="B29" s="76" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="78"/>
+      <c r="D29" s="80"/>
       <c r="E29" s="83"/>
       <c r="F29" s="83"/>
       <c r="G29" s="46"/>
     </row>
     <row r="30" spans="1:7" s="42" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="79"/>
+      <c r="A30" s="81"/>
       <c r="B30" s="76" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="79"/>
+      <c r="D30" s="81"/>
       <c r="E30" s="84"/>
       <c r="F30" s="84"/>
       <c r="G30" s="46"/>
@@ -1850,10 +1850,10 @@
       <c r="D31" s="41">
         <v>1</v>
       </c>
-      <c r="E31" s="85">
+      <c r="E31" s="77">
         <v>1020</v>
       </c>
-      <c r="F31" s="86">
+      <c r="F31" s="78">
         <f>E31*D31</f>
         <v>1020</v>
       </c>
@@ -1872,10 +1872,10 @@
       <c r="D32" s="41">
         <v>1</v>
       </c>
-      <c r="E32" s="85">
+      <c r="E32" s="77">
         <v>288</v>
       </c>
-      <c r="F32" s="86">
+      <c r="F32" s="78">
         <f>E32*D32</f>
         <v>288</v>
       </c>

</xml_diff>